<commit_message>
Actualizar datos de inventario y imagenes
</commit_message>
<xml_diff>
--- a/files/data/imagen.xlsx
+++ b/files/data/imagen.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yeison Mena\Desktop\vitalixplus-inventario-service\files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FAEDBF-F903-407C-B96E-567DCCF299F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D51C9E3-F49C-49EB-B4EB-A4674873662F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4395" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="imagen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>id_imagen</t>
   </si>
@@ -49,6 +60,174 @@
   </si>
   <si>
     <t>https://encrypted-tbn3.gstatic.com/shopping?q=tbn:ANd9GcSwMQKviqY6kGhEFe5uqHCCOikXw0VbOjfvMy5cGp8jXEq8_c0Myo5_XiSr-Jy1PMy9kIhvjNqwRQIv8nxvSec1kzRe1j7ICaIhoB2pHGFqyfqcW-w8J0DfqRM</t>
+  </si>
+  <si>
+    <t>https://share.google/images/8eM1Y9EGEKGyzBxZt</t>
+  </si>
+  <si>
+    <t>https://share.google/images/oRpF2pLbKLXljsHQr</t>
+  </si>
+  <si>
+    <t>https://share.google/images/HI9tEzSAbaModDLrB</t>
+  </si>
+  <si>
+    <t>https://share.google/images/XnX5BI93ii11MTGMX</t>
+  </si>
+  <si>
+    <t>https://share.google/images/qFEH9DA5PsbRgL4sM</t>
+  </si>
+  <si>
+    <t>https://share.google/images/U4RgJoNgiTOD8MkS4</t>
+  </si>
+  <si>
+    <t>https://share.google/images/AiEoli0RhQ1tSJa7E</t>
+  </si>
+  <si>
+    <t>https://share.google/images/JTUzL3CEUGlVGhkSH</t>
+  </si>
+  <si>
+    <t>https://share.google/images/1eDClsxuUvWO1RKCM</t>
+  </si>
+  <si>
+    <t>https://share.google/images/Hq9QeLxBK8UyXpceO</t>
+  </si>
+  <si>
+    <t>https://share.google/images/wR18V0WZ8IS174CTt</t>
+  </si>
+  <si>
+    <t>https://share.google/images/jDpQ4KcLQenVwBnOG</t>
+  </si>
+  <si>
+    <t>https://share.google/images/e4kOQNTlltIVFlkAw</t>
+  </si>
+  <si>
+    <t>https://share.google/images/TG41QpswAvkC4EgPV</t>
+  </si>
+  <si>
+    <t>https://share.google/images/mB5tHbNJiyQvynxlc</t>
+  </si>
+  <si>
+    <t>https://share.google/images/qwrrENyTO7LF1Kotc</t>
+  </si>
+  <si>
+    <t>https://share.google/images/iPhcX5Eu8gJcbDu1F</t>
+  </si>
+  <si>
+    <t>https://share.google/images/2qfP0OtnliAxCtQLP</t>
+  </si>
+  <si>
+    <t>https://share.google/images/w4HhDpGR00AzhjGnu</t>
+  </si>
+  <si>
+    <t>https://share.google/images/PSBHhHRSGk7uGrcKC</t>
+  </si>
+  <si>
+    <t>https://share.google/images/we4u7w5oDldpHv5DL</t>
+  </si>
+  <si>
+    <t>https://share.google/images/NLi7BD7cSmdw6T7vA</t>
+  </si>
+  <si>
+    <t>https://share.google/images/ByQHJcNOSqx8M7qLg</t>
+  </si>
+  <si>
+    <t>https://share.google/images/tdDmSB3BYlBHMR5pQ</t>
+  </si>
+  <si>
+    <t>https://share.google/images/pdfck8wKIQLpnWKcL</t>
+  </si>
+  <si>
+    <t>https://share.google/images/ZBlGs50c2NWKcSuS5</t>
+  </si>
+  <si>
+    <t>https://share.google/images/b7BAfKQxpBRaQeqWE</t>
+  </si>
+  <si>
+    <t>https://share.google/images/i3oavGqleJV8Ejw3C</t>
+  </si>
+  <si>
+    <t>https://share.google/images/GNO2Tu4BBnfCx8Pvq</t>
+  </si>
+  <si>
+    <t>https://share.google/images/sCdJROUFK35b8smVW</t>
+  </si>
+  <si>
+    <t>https://share.google/images/zlaqbBPpQtwKt74k9</t>
+  </si>
+  <si>
+    <t>https://share.google/images/JIP7bIO77CXBiI9sn</t>
+  </si>
+  <si>
+    <t>https://share.google/images/MLVlFglfn1xYlXZrI</t>
+  </si>
+  <si>
+    <t>https://share.google/images/fdj4Oip71rAAyD3bL</t>
+  </si>
+  <si>
+    <t>https://share.google/images/g4Uh1NMJ5O1JaOKMz</t>
+  </si>
+  <si>
+    <t>https://share.google/images/7CTPBUt70iy9Qam40</t>
+  </si>
+  <si>
+    <t>https://share.google/images/VryA3VUaw5O8M9PrP</t>
+  </si>
+  <si>
+    <t>https://share.google/images/Wqzm3CUYafNeYyiMq</t>
+  </si>
+  <si>
+    <t>https://share.google/images/eEJK9PhfrmJSM6oWF</t>
+  </si>
+  <si>
+    <t>https://share.google/images/6VS9Rq8cAQCZ0i7xz</t>
+  </si>
+  <si>
+    <t>https://share.google/images/qIpnlSQhTqlKL6in6</t>
+  </si>
+  <si>
+    <t>https://share.google/images/IyiMy4vuSXAhD8dNR</t>
+  </si>
+  <si>
+    <t>https://share.google/images/jgwsMbphPHjTlFyUd</t>
+  </si>
+  <si>
+    <t>https://share.google/images/UpuNIbqnsNOHBFd41</t>
+  </si>
+  <si>
+    <t>https://share.google/images/xQY5yocBtYHDhtHCK</t>
+  </si>
+  <si>
+    <t>https://share.google/images/jw7BdsHPb7NmsUu0m</t>
+  </si>
+  <si>
+    <t>https://share.google/images/8ylKS3LQsqXtqcH8x</t>
+  </si>
+  <si>
+    <t>https://share.google/images/q3YeIncl7JKJWbe7k</t>
+  </si>
+  <si>
+    <t>https://share.google/images/ZT4OFA6kTfuaQeeni</t>
+  </si>
+  <si>
+    <t>https://share.google/images/bMdikqEtfHMVbK2oX</t>
+  </si>
+  <si>
+    <t>https://share.google/images/RyssLhAsTKJyxnWyU</t>
+  </si>
+  <si>
+    <t>https://share.google/images/rcSsiH9nVSxPjLS18</t>
+  </si>
+  <si>
+    <t>https://share.google/images/dSLxHXwJtMtSM3hBi</t>
+  </si>
+  <si>
+    <t>https://share.google/images/UZo4u4dpjHi4liAtN</t>
+  </si>
+  <si>
+    <t>https://share.google/images/I4M3WvdmaCEwYTuHT</t>
+  </si>
+  <si>
+    <t>https://share.google/images/NY7QQId6eli15Fcxt</t>
   </si>
 </sst>
 </file>
@@ -124,8 +303,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7450E731-C284-474F-B115-531F72DAE462}" name="imagen" displayName="imagen" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6" xr:uid="{7450E731-C284-474F-B115-531F72DAE462}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7450E731-C284-474F-B115-531F72DAE462}" name="imagen" displayName="imagen" ref="A1:C64" totalsRowShown="0">
+  <autoFilter ref="A1:C64" xr:uid="{7450E731-C284-474F-B115-531F72DAE462}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EB4D1AAA-C9B5-41CB-92F4-C4AA5A191094}" name="id_imagen"/>
     <tableColumn id="2" xr3:uid="{D57247A9-017A-439A-98A4-6FB2011C2D61}" name="Código"/>
@@ -398,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +653,644 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>55104</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>54445</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>56184</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>54023</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>55927</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>55947</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>54902</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>53990</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>54839</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>55375</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>55307</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>55202</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>55914</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>56157</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>56058</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>55829</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>55830</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>55330</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>55315</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>53872</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>54823</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>54822</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>55950</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>54944</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>54332</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>55989</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>56146</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>55509</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>56111</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>55541</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>55650</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>54846</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>54123</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>55781</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>54529</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>54615</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>55788</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>55939</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>54569</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>55938</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>54294</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>54740</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>55907</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>55911</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>55912</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>55910</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>55909</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>55908</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>54493</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>54937</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>55714</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>55806</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>56169</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>55095</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>54725</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>55269</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>54990</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>55867</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>